<commit_message>
create biaya pendaftaran, spp, bpp
</commit_message>
<xml_diff>
--- a/progres.xlsx
+++ b/progres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\server\www\pemograman-web-2-pmb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A571806B-485B-4E84-92F6-E2EF7FD037DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFAE6AE-C44A-442B-A273-08123487ADA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>NO</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Periode</t>
+  </si>
+  <si>
+    <t>Pendaftaran</t>
+  </si>
+  <si>
+    <t>BPP</t>
+  </si>
+  <si>
+    <t>SPP</t>
   </si>
 </sst>
 </file>
@@ -117,16 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -411,7 +417,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +445,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -454,7 +460,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="5"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -486,34 +492,40 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">

</xml_diff>